<commit_message>
updated wrangling, modified xlsx files
</commit_message>
<xml_diff>
--- a/data/bacterial-metabolites_dose-simicillin_long.xlsx
+++ b/data/bacterial-metabolites_dose-simicillin_long.xlsx
@@ -1,21 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffsocal/Local/github/ASMS_R_Basics/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{335E0C3B-DB0A-AB48-85C3-51333FD2D3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="20">
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Metabolite</t>
+  </si>
+  <si>
+    <t>Time_0min</t>
+  </si>
+  <si>
+    <t>Time_10min</t>
+  </si>
+  <si>
+    <t>Time_20min</t>
+  </si>
+  <si>
+    <t>Time_50min</t>
+  </si>
+  <si>
+    <t>Time_2hr</t>
+  </si>
+  <si>
+    <t>e coli dose:0mg</t>
+  </si>
+  <si>
+    <t>glutamate</t>
+  </si>
+  <si>
+    <t>staph aureus dose:0mg</t>
+  </si>
+  <si>
+    <t>p aeruginosa dose:0mg</t>
+  </si>
+  <si>
+    <t>e coli dose:10mg</t>
+  </si>
+  <si>
+    <t>staph aureus dose:10mg</t>
+  </si>
+  <si>
+    <t>p aeruginosa dose:10mg</t>
+  </si>
+  <si>
+    <t>e coli dose:20mg</t>
+  </si>
+  <si>
+    <t>staph aureus dose:20mg</t>
+  </si>
+  <si>
+    <t>p aeruginosa dose:20mg</t>
+  </si>
+  <si>
+    <t>lysine</t>
+  </si>
+  <si>
+    <t>succinic acid</t>
+  </si>
+  <si>
+    <t>phosphatidylcholine</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +134,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +186,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +220,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +255,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,60 +431,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Culture</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Metabolite</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Time_0min</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Time_10min</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Time_20min</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Time_50min</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Time_2hr</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>e coli dose:0mg</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>glutamate</t>
-        </is>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>191666</v>
@@ -421,16 +484,12 @@
         <v>1782879</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>staph aureus dose:0mg</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>glutamate</t>
-        </is>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3">
         <v>125210</v>
@@ -448,16 +507,12 @@
         <v>137747</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:0mg</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>glutamate</t>
-        </is>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
       <c r="C4">
         <v>978126</v>
@@ -475,16 +530,12 @@
         <v>1630613</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>e coli dose:10mg</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>glutamate</t>
-        </is>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
       <c r="C5">
         <v>1445</v>
@@ -502,16 +553,12 @@
         <v>29825</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>staph aureus dose:10mg</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>glutamate</t>
-        </is>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
       <c r="C6">
         <v>152</v>
@@ -529,16 +576,12 @@
         <v>10920</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:10mg</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>glutamate</t>
-        </is>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
       </c>
       <c r="C7">
         <v>23</v>
@@ -556,16 +599,12 @@
         <v>230032</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>e coli dose:20mg</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>glutamate</t>
-        </is>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
       </c>
       <c r="C8">
         <v>885</v>
@@ -583,16 +622,12 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>staph aureus dose:20mg</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>glutamate</t>
-        </is>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
       </c>
       <c r="C9">
         <v>136</v>
@@ -610,16 +645,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:20mg</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>glutamate</t>
-        </is>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
       </c>
       <c r="C10">
         <v>3098</v>
@@ -637,16 +668,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>e coli dose:0mg</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
       </c>
       <c r="C11">
         <v>1418</v>
@@ -664,16 +691,12 @@
         <v>962</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>staph aureus dose:0mg</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
       </c>
       <c r="C12">
         <v>111</v>
@@ -691,16 +714,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:0mg</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
       </c>
       <c r="C13">
         <v>15</v>
@@ -718,16 +737,12 @@
         <v>861</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>e coli dose:10mg</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
       </c>
       <c r="C14">
         <v>1830</v>
@@ -745,16 +760,12 @@
         <v>179472</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>staph aureus dose:10mg</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
       </c>
       <c r="C15">
         <v>137</v>
@@ -772,16 +783,12 @@
         <v>12885</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:10mg</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
       </c>
       <c r="C16">
         <v>3705</v>
@@ -799,16 +806,12 @@
         <v>136535</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>e coli dose:20mg</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
       </c>
       <c r="C17">
         <v>367</v>
@@ -826,16 +829,12 @@
         <v>187863</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>staph aureus dose:20mg</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
       </c>
       <c r="C18">
         <v>129</v>
@@ -853,16 +852,12 @@
         <v>1458806</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:20mg</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
       </c>
       <c r="C19">
         <v>3067</v>
@@ -880,16 +875,12 @@
         <v>22340479</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>e coli dose:0mg</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>succinic acid</t>
-        </is>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
       </c>
       <c r="C20">
         <v>1678885</v>
@@ -907,16 +898,12 @@
         <v>173066</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>staph aureus dose:0mg</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>succinic acid</t>
-        </is>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
       </c>
       <c r="C21">
         <v>110418</v>
@@ -934,16 +921,12 @@
         <v>109675</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:0mg</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>succinic acid</t>
-        </is>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
       </c>
       <c r="C22">
         <v>2558815</v>
@@ -961,16 +944,12 @@
         <v>794206</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>e coli dose:10mg</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>succinic acid</t>
-        </is>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
       </c>
       <c r="C23">
         <v>50501</v>
@@ -988,16 +967,12 @@
         <v>212618</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>staph aureus dose:10mg</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>succinic acid</t>
-        </is>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
       </c>
       <c r="C24">
         <v>11442</v>
@@ -1015,16 +990,12 @@
         <v>13058</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:10mg</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>succinic acid</t>
-        </is>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
       </c>
       <c r="C25">
         <v>101008</v>
@@ -1042,16 +1013,12 @@
         <v>40676</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>e coli dose:20mg</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>succinic acid</t>
-        </is>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
       </c>
       <c r="C26">
         <v>186375</v>
@@ -1069,16 +1036,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>staph aureus dose:20mg</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>succinic acid</t>
-        </is>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
       </c>
       <c r="C27">
         <v>11769</v>
@@ -1096,16 +1059,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:20mg</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>succinic acid</t>
-        </is>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
       </c>
       <c r="C28">
         <v>198848</v>
@@ -1123,16 +1082,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>e coli dose:0mg</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>phosphatidylcholine</t>
-        </is>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
       </c>
       <c r="C29">
         <v>84588958</v>
@@ -1150,16 +1105,12 @@
         <v>175507910</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>staph aureus dose:0mg</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>phosphatidylcholine</t>
-        </is>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
       </c>
       <c r="C30">
         <v>14739821</v>
@@ -1177,16 +1128,12 @@
         <v>11830920</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:0mg</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>phosphatidylcholine</t>
-        </is>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
       </c>
       <c r="C31">
         <v>93496213</v>
@@ -1204,16 +1151,12 @@
         <v>120335903</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>e coli dose:10mg</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>phosphatidylcholine</t>
-        </is>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
       </c>
       <c r="C32">
         <v>128103670</v>
@@ -1231,16 +1174,12 @@
         <v>118321</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>staph aureus dose:10mg</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>phosphatidylcholine</t>
-        </is>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
       </c>
       <c r="C33">
         <v>9935549</v>
@@ -1258,16 +1197,12 @@
         <v>12694</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:10mg</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>phosphatidylcholine</t>
-        </is>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
       </c>
       <c r="C34">
         <v>326068174</v>
@@ -1285,16 +1220,12 @@
         <v>8778</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>e coli dose:20mg</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>phosphatidylcholine</t>
-        </is>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
       </c>
       <c r="C35">
         <v>183210138</v>
@@ -1312,16 +1243,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>staph aureus dose:20mg</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>phosphatidylcholine</t>
-        </is>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
       </c>
       <c r="C36">
         <v>10982763</v>
@@ -1339,16 +1266,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>p aeruginosa dose:20mg</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>phosphatidylcholine</t>
-        </is>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
       </c>
       <c r="C37">
         <v>101693193</v>

</xml_diff>